<commit_message>
corrected typo in resistor value
</commit_message>
<xml_diff>
--- a/BOM/darpa-power-distribution-BOM.xlsx
+++ b/BOM/darpa-power-distribution-BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="13620" windowHeight="5070"/>
+    <workbookView activeTab="0" windowWidth="13620" windowHeight="5080"/>
   </bookViews>
   <sheets>
     <sheet name="darpa-power-distribution-raw.csv" sheetId="1" r:id="rId1"/>
@@ -19,28 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31" count="31">
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Package</t>
-  </si>
-  <si>
-    <t>Parts</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>POPULARITY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24" count="24">
   <si>
     <t>M251</t>
   </si>
@@ -188,7 +167,7 @@
   <dimension ref="A1:IV34"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -200,30 +179,44 @@
     <col min="5" max="5" style="0" width="68.5673076923077" customWidth="1"/>
     <col min="6" max="6" style="0" width="53.56820913461539" customWidth="1"/>
     <col min="7" max="7" style="0" width="12.284975961538462" customWidth="1"/>
-    <col min="8" max="256" style="0" width="9.142307692307693"/>
+    <col min="8" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Device</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Package</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Parts</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>POPULARITY</t>
+        </is>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -533,10 +526,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -584,10 +577,10 @@
         </is>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -595,7 +588,7 @@
         </is>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <v>52</v>
@@ -611,10 +604,10 @@
         </is>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -622,7 +615,7 @@
         </is>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G7">
         <v>86</v>
@@ -638,10 +631,10 @@
         </is>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -649,7 +642,7 @@
         </is>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <v>52</v>
@@ -665,10 +658,10 @@
         </is>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -676,7 +669,7 @@
         </is>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <v>86</v>
@@ -707,7 +700,7 @@
         </is>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G10">
         <v>12</v>
@@ -723,10 +716,10 @@
         </is>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -734,7 +727,7 @@
         </is>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <v>52</v>
@@ -750,10 +743,10 @@
         </is>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -761,7 +754,7 @@
         </is>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <v>86</v>
@@ -775,10 +768,10 @@
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -786,7 +779,7 @@
         </is>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G13">
         <v>86</v>
@@ -817,7 +810,7 @@
         </is>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -833,10 +826,10 @@
         </is>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -844,7 +837,7 @@
         </is>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G15">
         <v>26</v>
@@ -860,10 +853,10 @@
         </is>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -871,7 +864,7 @@
         </is>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:256" ht="13.5">
@@ -884,10 +877,10 @@
         </is>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -895,7 +888,7 @@
         </is>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:256">
@@ -906,10 +899,10 @@
         <v>470</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -917,7 +910,7 @@
         </is>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G18">
         <v>86</v>
@@ -948,7 +941,7 @@
         </is>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G19">
         <v>4</v>
@@ -964,10 +957,10 @@
         </is>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -975,24 +968,26 @@
         </is>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G20">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:256">
+    <row r="21" spans="1:256" ht="13.5">
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21">
-        <v>5.2300000000000004</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>5.23k</t>
+        </is>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1000,7 +995,7 @@
         </is>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G21">
         <v>86</v>
@@ -1016,10 +1011,10 @@
         </is>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1027,7 +1022,7 @@
         </is>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G22">
         <v>86</v>
@@ -1041,10 +1036,10 @@
         <v>600</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1052,7 +1047,7 @@
         </is>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G23">
         <v>86</v>
@@ -1092,10 +1087,10 @@
         </is>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1103,7 +1098,7 @@
         </is>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G25">
         <v>86</v>
@@ -1114,13 +1109,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1138,13 +1133,13 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1162,10 +1157,10 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1191,13 +1186,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1210,13 +1205,13 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1234,10 +1229,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1260,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1279,13 +1274,13 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1298,13 +1293,13 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1312,7 +1307,7 @@
         </is>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>